<commit_message>
Adicionei as condições de contorno
</commit_message>
<xml_diff>
--- a/entrada_aps3.xlsx
+++ b/entrada_aps3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferna\Documents\Insper\5semestre\Tranferência de calor e mecânica dos sólidos\mecsol-APS3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6E9A64-1EA1-488B-BFF1-97E0D9463153}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB22361-EF52-4919-BAE5-AC4E1F71BB58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8610" yWindow="1800" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nos" sheetId="1" r:id="rId1"/>
@@ -509,7 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>